<commit_message>
Update v9 final for fall
Changed map rankings to new rankings, ran webscraper 12/6
</commit_message>
<xml_diff>
--- a/MapandSearchFunder/output.xlsx
+++ b/MapandSearchFunder/output.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -948,13 +948,13 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.7272727272727273</v>
+        <v>0.8181818181818182</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>0.2727272727272727</v>
+        <v>0.1818181818181818</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
@@ -998,22 +998,22 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.72</v>
+        <v>0.7333333333333333</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>0.28</v>
+        <v>0.2333333333333333</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="G23" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24">
@@ -1023,22 +1023,22 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.6333333333333333</v>
+        <v>0.6129032258064516</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>0.3666666666666666</v>
+        <v>0.3548387096774194</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>0</v>
+        <v>0.03225806451612903</v>
       </c>
       <c r="G24" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25">
@@ -1098,22 +1098,22 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.6451612903225806</v>
+        <v>0.6363636363636364</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>0.2903225806451613</v>
+        <v>0.2727272727272727</v>
       </c>
       <c r="E27" t="n">
-        <v>0.03225806451612903</v>
+        <v>0.0303030303030303</v>
       </c>
       <c r="F27" t="n">
-        <v>0.03225806451612903</v>
+        <v>0.06060606060606061</v>
       </c>
       <c r="G27" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28">
@@ -1148,22 +1148,22 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.5925925925925926</v>
+        <v>0.6024096385542169</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>0.2345679012345679</v>
+        <v>0.2168674698795181</v>
       </c>
       <c r="E29" t="n">
-        <v>0.01234567901234568</v>
+        <v>0.01204819277108434</v>
       </c>
       <c r="F29" t="n">
-        <v>0.1604938271604938</v>
+        <v>0.1686746987951807</v>
       </c>
       <c r="G29" t="n">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30">
@@ -1173,22 +1173,22 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.5730337078651685</v>
+        <v>0.5824175824175825</v>
       </c>
       <c r="C30" t="n">
-        <v>0.03370786516853932</v>
+        <v>0.03296703296703297</v>
       </c>
       <c r="D30" t="n">
-        <v>0.303370786516854</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="E30" t="n">
         <v>0</v>
       </c>
       <c r="F30" t="n">
-        <v>0.0898876404494382</v>
+        <v>0.0989010989010989</v>
       </c>
       <c r="G30" t="n">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31">
@@ -1198,7 +1198,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.6058394160583942</v>
+        <v>0.6131386861313869</v>
       </c>
       <c r="C31" t="n">
         <v>0.0218978102189781</v>
@@ -1210,7 +1210,7 @@
         <v>0.0218978102189781</v>
       </c>
       <c r="F31" t="n">
-        <v>0.2262773722627737</v>
+        <v>0.218978102189781</v>
       </c>
       <c r="G31" t="n">
         <v>137</v>
@@ -1223,22 +1223,22 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.463768115942029</v>
+        <v>0.4951456310679612</v>
       </c>
       <c r="C32" t="n">
-        <v>0.02415458937198068</v>
+        <v>0.01941747572815534</v>
       </c>
       <c r="D32" t="n">
-        <v>0.106280193236715</v>
+        <v>0.1067961165048544</v>
       </c>
       <c r="E32" t="n">
-        <v>0.00966183574879227</v>
+        <v>0.009708737864077669</v>
       </c>
       <c r="F32" t="n">
-        <v>0.3961352657004831</v>
+        <v>0.3689320388349515</v>
       </c>
       <c r="G32" t="n">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="33">
@@ -1248,22 +1248,22 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.2741935483870968</v>
+        <v>0.305</v>
       </c>
       <c r="C33" t="n">
-        <v>0.07526881720430108</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="D33" t="n">
-        <v>0.03763440860215054</v>
+        <v>0.05</v>
       </c>
       <c r="E33" t="n">
-        <v>0.07526881720430108</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="F33" t="n">
-        <v>0.5376344086021505</v>
+        <v>0.505</v>
       </c>
       <c r="G33" t="n">
-        <v>186</v>
+        <v>200</v>
       </c>
     </row>
     <row r="34">
@@ -1273,22 +1273,22 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.1541353383458647</v>
+        <v>0.2202797202797203</v>
       </c>
       <c r="C34" t="n">
-        <v>0.1240601503759398</v>
+        <v>0.1048951048951049</v>
       </c>
       <c r="D34" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01748251748251748</v>
       </c>
       <c r="E34" t="n">
-        <v>0.112781954887218</v>
+        <v>0.0944055944055944</v>
       </c>
       <c r="F34" t="n">
-        <v>0.5939849624060151</v>
+        <v>0.5629370629370629</v>
       </c>
       <c r="G34" t="n">
-        <v>266</v>
+        <v>286</v>
       </c>
     </row>
     <row r="35">
@@ -1298,22 +1298,22 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.05120481927710843</v>
+        <v>0.1201044386422977</v>
       </c>
       <c r="C35" t="n">
-        <v>0.1837349397590362</v>
+        <v>0.1462140992167102</v>
       </c>
       <c r="D35" t="n">
-        <v>0.009036144578313253</v>
+        <v>0.01044386422976501</v>
       </c>
       <c r="E35" t="n">
-        <v>0.1114457831325301</v>
+        <v>0.1044386422976501</v>
       </c>
       <c r="F35" t="n">
-        <v>0.6445783132530121</v>
+        <v>0.618798955613577</v>
       </c>
       <c r="G35" t="n">
-        <v>332</v>
+        <v>383</v>
       </c>
     </row>
     <row r="36">
@@ -1323,22 +1323,47 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.008849557522123894</v>
+        <v>0.01937984496124031</v>
       </c>
       <c r="C36" t="n">
-        <v>0.1504424778761062</v>
+        <v>0.08139534883720931</v>
       </c>
       <c r="D36" t="n">
-        <v>0</v>
+        <v>0.007751937984496124</v>
       </c>
       <c r="E36" t="n">
-        <v>0.2123893805309734</v>
+        <v>0.07751937984496124</v>
       </c>
       <c r="F36" t="n">
-        <v>0.6283185840707964</v>
+        <v>0.813953488372093</v>
       </c>
       <c r="G36" t="n">
-        <v>113</v>
+        <v>258</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>